<commit_message>
Driver manager, extent reports updates
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestCases.xlsx
+++ b/src/test/resources/data/TestCases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>testname</t>
   </si>
@@ -59,10 +59,13 @@
     <t>no</t>
   </si>
   <si>
-    <t>Prathap</t>
-  </si>
-  <si>
     <t>test3</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>ABCD</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -462,16 +465,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -524,7 +521,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>

</xml_diff>